<commit_message>
Modify the functionalities in page ShareSkill
</commit_message>
<xml_diff>
--- a/marsframework-master/MarsFramework/ExcelData/TestData.xlsx
+++ b/marsframework-master/MarsFramework/ExcelData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23405"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhya\Downloads\MarsFramework\MarsFramework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B780BCC1-12AA-401B-9859-0747B9498333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD9D716F-43E3-4E17-9CDB-478C0D14E8F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>FirstName</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Credit</t>
+  </si>
+  <si>
+    <t>CreditAmount</t>
   </si>
   <si>
     <t>Active</t>
@@ -731,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A4F2D9-8930-471B-B711-C6320281A763}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -751,6 +754,7 @@
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -802,38 +806,40 @@
       <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H2" s="5">
-        <v>43567</v>
+        <v>44298</v>
       </c>
       <c r="I2" s="6">
-        <v>43597</v>
+        <v>44328</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K2" s="7">
         <v>0.75</v>
@@ -845,13 +851,16 @@
         <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O2" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="s">
-        <v>36</v>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -878,7 +887,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -898,10 +907,10 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -918,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -936,31 +945,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -968,34 +977,34 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add assertion on test cases
</commit_message>
<xml_diff>
--- a/marsframework-master/MarsFramework/ExcelData/TestData.xlsx
+++ b/marsframework-master/MarsFramework/ExcelData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhya\Downloads\MarsFramework\MarsFramework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD9D716F-43E3-4E17-9CDB-478C0D14E8F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E50ED6F4-28A3-4388-99C7-C8E5989B84DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,9 +218,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -279,7 +280,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -288,6 +289,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -735,7 +738,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -832,10 +835,10 @@
       <c r="G2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="8">
         <v>44298</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="9">
         <v>44328</v>
       </c>
       <c r="J2" s="6" t="s">

</xml_diff>